<commit_message>
* fix import auto-filter issue * add more test cases for it
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/filter.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/filter.xlsx
@@ -4,22 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="19155" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="19155" windowHeight="7740" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Filter1" sheetId="1" r:id="rId1"/>
-    <sheet name="Filter2" sheetId="2" r:id="rId2"/>
+    <sheet name="1 column" sheetId="1" r:id="rId1"/>
+    <sheet name="2 columns" sheetId="2" r:id="rId2"/>
+    <sheet name="no criteria" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Filter1!$B$1:$D$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Filter2!$A$1:$C$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1 column'!$B$1:$D$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2 columns'!$A$1:$C$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'no criteria'!$B$2:$D$11</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="21">
   <si>
     <t>Type</t>
   </si>
@@ -507,8 +509,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -561,7 +563,7 @@
         <v>6328</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="17.25" hidden="1" thickBot="1">
+    <row r="5" spans="2:4" ht="17.25" thickBot="1">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -594,7 +596,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="17.25" thickBot="1">
+    <row r="8" spans="2:4" ht="17.25" hidden="1" thickBot="1">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -629,9 +631,9 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:D10">
-    <filterColumn colId="0">
+    <filterColumn colId="1">
       <filters>
-        <filter val="Meat"/>
+        <filter val="Davolio"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -906,4 +908,136 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6328</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6544</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="17.25" thickBot="1">
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2150</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:D11"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>